<commit_message>
Add feature RetryAnalyzer for failed test case
</commit_message>
<xml_diff>
--- a/testData/loginData.xlsx
+++ b/testData/loginData.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ShopingWebSiteProject\ShoppingWebsite-Automation-Framework\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99B29FE3-26CE-4617-8560-B077C982B571}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB537CA1-492A-4222-82B9-FCEBE6297919}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginTestData" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,43 +25,28 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="4">
-  <si>
-    <t>emailAddress</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
   <si>
     <t>password</t>
   </si>
   <si>
-    <t>rehankhan56390@gmail.com</t>
+    <t>angelatucker13287@suffermail.com</t>
   </si>
   <si>
-    <t>angelatucker13287@suffermail.com</t>
+    <t>emailAddress</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF859900"/>
-      <name val="Consolas"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF2AA198"/>
-      <name val="Consolas"/>
-      <family val="3"/>
     </font>
     <font>
       <u/>
@@ -91,13 +76,11 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -379,65 +362,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.77734375" customWidth="1"/>
-    <col min="2" max="2" width="8.33203125" customWidth="1"/>
+    <col min="1" max="1" width="35.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="3" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2">
-        <v>12345</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2">
-        <v>12345</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="2">
-        <v>12345</v>
+      <c r="B2" t="s">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1" xr:uid="{FC122915-4FD2-45B0-B400-8BE2C8BD0198}"/>
-    <hyperlink ref="A4:A5" r:id="rId2" display="rehankhan56390@gmail.com" xr:uid="{4107B5B9-FFC1-4CCC-942A-FAD734846444}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{BEB2B972-2302-40B9-9D1C-75AE13066ACC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>